<commit_message>
all good example_multiple_strats + good folders to save results
</commit_message>
<xml_diff>
--- a/results/final_results/metrics/all_metrics.xlsx
+++ b/results/final_results/metrics/all_metrics.xlsx
@@ -1162,436 +1162,436 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.492087951848628</v>
+        <v>1.061178901566156</v>
       </c>
       <c r="C2" t="n">
-        <v>2.492087951848628</v>
+        <v>1.82334221379167</v>
       </c>
       <c r="D2" t="n">
-        <v>2.492087951848628</v>
+        <v>2.924212086940387</v>
       </c>
       <c r="E2" t="n">
-        <v>2.492087951848628</v>
+        <v>2.504747943975057</v>
       </c>
       <c r="F2" t="n">
-        <v>3.146294190546269</v>
+        <v>1.888377631694168</v>
       </c>
       <c r="G2" t="n">
-        <v>3.146294190546269</v>
+        <v>2.032095552961039</v>
       </c>
       <c r="H2" t="n">
-        <v>3.146294190546269</v>
+        <v>1.787542246203888</v>
       </c>
       <c r="I2" t="n">
-        <v>3.146294190546269</v>
+        <v>1.259161126550745</v>
       </c>
       <c r="J2" t="n">
-        <v>2.608486965426043</v>
+        <v>1.417593742320825</v>
       </c>
       <c r="K2" t="n">
-        <v>2.608486965426043</v>
+        <v>2.429525908024328</v>
       </c>
       <c r="L2" t="n">
-        <v>2.608486965426043</v>
+        <v>1.698822467259674</v>
       </c>
       <c r="M2" t="n">
-        <v>2.608486965426043</v>
+        <v>1.646165452559609</v>
       </c>
       <c r="N2" t="n">
-        <v>4.093838582178354</v>
+        <v>2.238048955574774</v>
       </c>
       <c r="O2" t="n">
-        <v>4.093838582178354</v>
+        <v>1.476408831168503</v>
       </c>
       <c r="P2" t="n">
-        <v>4.093838582178354</v>
+        <v>1.683181110795882</v>
       </c>
       <c r="Q2" t="n">
-        <v>4.093838582178354</v>
+        <v>2.212863786910388</v>
       </c>
       <c r="R2" t="n">
-        <v>2.769233054757132</v>
+        <v>1.410638390910292</v>
       </c>
       <c r="S2" t="n">
-        <v>2.769233054757132</v>
+        <v>2.067675760473938</v>
       </c>
       <c r="T2" t="n">
-        <v>2.769233054757132</v>
+        <v>1.402520515108208</v>
       </c>
       <c r="U2" t="n">
-        <v>2.769233054757132</v>
+        <v>1.561801680626045</v>
       </c>
       <c r="V2" t="n">
-        <v>3.957493580185496</v>
+        <v>2.036452820393287</v>
       </c>
       <c r="W2" t="n">
-        <v>3.957493580185496</v>
+        <v>1.716675828919638</v>
       </c>
       <c r="X2" t="n">
-        <v>3.957493580185496</v>
+        <v>2.170331355664562</v>
       </c>
       <c r="Y2" t="n">
-        <v>3.957493580185496</v>
+        <v>2.750510557344534</v>
       </c>
       <c r="Z2" t="n">
-        <v>8.419828913033111</v>
+        <v>6.599086400253861</v>
       </c>
       <c r="AA2" t="n">
-        <v>8.419828913033111</v>
+        <v>3.493372706751606</v>
       </c>
       <c r="AB2" t="n">
-        <v>8.419828913033111</v>
+        <v>1.928477972331316</v>
       </c>
       <c r="AC2" t="n">
-        <v>8.419828913033111</v>
+        <v>3.416016559236335</v>
       </c>
       <c r="AD2" t="n">
-        <v>4.595316747163769</v>
+        <v>3.694689130068658</v>
       </c>
       <c r="AE2" t="n">
-        <v>4.595316747163769</v>
+        <v>2.44387160170255</v>
       </c>
       <c r="AF2" t="n">
-        <v>4.595316747163769</v>
+        <v>1.674070330684425</v>
       </c>
       <c r="AG2" t="n">
-        <v>4.595316747163769</v>
+        <v>2.19938850292108</v>
       </c>
       <c r="AH2" t="n">
-        <v>4.953039512837357</v>
+        <v>3.970273092274673</v>
       </c>
       <c r="AI2" t="n">
-        <v>4.953039512837357</v>
+        <v>2.188827807692037</v>
       </c>
       <c r="AJ2" t="n">
-        <v>4.953039512837357</v>
+        <v>1.654143949432997</v>
       </c>
       <c r="AK2" t="n">
-        <v>4.953039512837357</v>
+        <v>1.687607920236002</v>
       </c>
       <c r="AL2" t="n">
-        <v>3.892984052012319</v>
+        <v>3.228519216870875</v>
       </c>
       <c r="AM2" t="n">
-        <v>3.892984052012319</v>
+        <v>2.222494140688087</v>
       </c>
       <c r="AN2" t="n">
-        <v>3.892984052012319</v>
+        <v>1.666522121822827</v>
       </c>
       <c r="AO2" t="n">
-        <v>3.892984052012319</v>
+        <v>2.226898811446031</v>
       </c>
       <c r="AP2" t="n">
-        <v>4.756493123702352</v>
+        <v>3.650067298545854</v>
       </c>
       <c r="AQ2" t="n">
-        <v>4.756493123702352</v>
+        <v>2.597895887573114</v>
       </c>
       <c r="AR2" t="n">
-        <v>4.756493123702352</v>
+        <v>1.618670058081498</v>
       </c>
       <c r="AS2" t="n">
-        <v>4.756493123702352</v>
+        <v>1.963717017619762</v>
       </c>
       <c r="AT2" t="n">
-        <v>3.048826966925728</v>
+        <v>2.629423881492796</v>
       </c>
       <c r="AU2" t="n">
-        <v>3.048826966925728</v>
+        <v>1.978597735822341</v>
       </c>
       <c r="AV2" t="n">
-        <v>3.048826966925728</v>
+        <v>1.387327700933589</v>
       </c>
       <c r="AW2" t="n">
-        <v>3.048826966925728</v>
+        <v>2.078861322634379</v>
       </c>
       <c r="AX2" t="n">
-        <v>7.031838502882168</v>
+        <v>3.107514104694014</v>
       </c>
       <c r="AY2" t="n">
-        <v>7.031838502882168</v>
+        <v>2.331109313891435</v>
       </c>
       <c r="AZ2" t="n">
-        <v>7.031838502882168</v>
+        <v>3.584121095670191</v>
       </c>
       <c r="BA2" t="n">
-        <v>7.031838502882168</v>
+        <v>3.279888227450619</v>
       </c>
       <c r="BB2" t="n">
-        <v>12.56001733640849</v>
+        <v>5.659532655916158</v>
       </c>
       <c r="BC2" t="n">
-        <v>12.56001733640849</v>
+        <v>2.687466979650546</v>
       </c>
       <c r="BD2" t="n">
-        <v>12.56001733640849</v>
+        <v>2.195162109136188</v>
       </c>
       <c r="BE2" t="n">
-        <v>12.56001733640849</v>
+        <v>1.080040744618192</v>
       </c>
       <c r="BF2" t="n">
-        <v>8.655010061477739</v>
+        <v>4.041543410907276</v>
       </c>
       <c r="BG2" t="n">
-        <v>8.655010061477739</v>
+        <v>2.774904676929304</v>
       </c>
       <c r="BH2" t="n">
-        <v>8.655010061477739</v>
+        <v>2.4502190769265</v>
       </c>
       <c r="BI2" t="n">
-        <v>8.655010061477739</v>
+        <v>2.779279771802849</v>
       </c>
       <c r="BJ2" t="n">
-        <v>10.63383618164951</v>
+        <v>5.558004022275029</v>
       </c>
       <c r="BK2" t="n">
-        <v>10.63383618164951</v>
+        <v>3.201348955650891</v>
       </c>
       <c r="BL2" t="n">
-        <v>10.63383618164951</v>
+        <v>2.504005718847303</v>
       </c>
       <c r="BM2" t="n">
-        <v>10.63383618164951</v>
+        <v>1.548902890697653</v>
       </c>
       <c r="BN2" t="n">
-        <v>7.644994757638976</v>
+        <v>3.85828686644459</v>
       </c>
       <c r="BO2" t="n">
-        <v>7.644994757638976</v>
+        <v>2.396651658070254</v>
       </c>
       <c r="BP2" t="n">
-        <v>7.644994757638976</v>
+        <v>2.221027104144354</v>
       </c>
       <c r="BQ2" t="n">
-        <v>7.644994757638976</v>
+        <v>2.053768036451745</v>
       </c>
       <c r="BR2" t="n">
-        <v>8.739737523653844</v>
+        <v>4.512437007687559</v>
       </c>
       <c r="BS2" t="n">
-        <v>8.739737523653844</v>
+        <v>2.861094154219793</v>
       </c>
       <c r="BT2" t="n">
-        <v>8.739737523653844</v>
+        <v>2.095452248170827</v>
       </c>
       <c r="BU2" t="n">
-        <v>8.739737523653844</v>
+        <v>1.730313709472689</v>
       </c>
       <c r="BV2" t="n">
-        <v>3.255216394905959</v>
+        <v>1.713856309567261</v>
       </c>
       <c r="BW2" t="n">
-        <v>3.255216394905959</v>
+        <v>2.126293931837699</v>
       </c>
       <c r="BX2" t="n">
-        <v>3.255216394905959</v>
+        <v>1.222448860302668</v>
       </c>
       <c r="BY2" t="n">
-        <v>3.255216394905959</v>
+        <v>3.204737579535382</v>
       </c>
       <c r="BZ2" t="n">
-        <v>3.744591270921114</v>
+        <v>1.526598804542164</v>
       </c>
       <c r="CA2" t="n">
-        <v>3.744591270921114</v>
+        <v>1.141586518999498</v>
       </c>
       <c r="CB2" t="n">
-        <v>3.744591270921114</v>
+        <v>0.7693298631982859</v>
       </c>
       <c r="CC2" t="n">
-        <v>3.744591270921114</v>
+        <v>2.476056754324119</v>
       </c>
       <c r="CD2" t="n">
-        <v>5.410806963442114</v>
+        <v>3.089399738459683</v>
       </c>
       <c r="CE2" t="n">
-        <v>5.410806963442114</v>
+        <v>0.9624011344622343</v>
       </c>
       <c r="CF2" t="n">
-        <v>5.410806963442114</v>
+        <v>0.6143673391598241</v>
       </c>
       <c r="CG2" t="n">
-        <v>5.410806963442114</v>
+        <v>3.272346207146099</v>
       </c>
       <c r="CH2" t="n">
-        <v>3.628690556795216</v>
+        <v>1.504146026793536</v>
       </c>
       <c r="CI2" t="n">
-        <v>3.628690556795216</v>
+        <v>1.662507430258918</v>
       </c>
       <c r="CJ2" t="n">
-        <v>3.628690556795216</v>
+        <v>0.653773254373571</v>
       </c>
       <c r="CK2" t="n">
-        <v>3.628690556795216</v>
+        <v>1.74316285680514</v>
       </c>
       <c r="CL2" t="n">
-        <v>8.235916268216402</v>
+        <v>4.888287108202757</v>
       </c>
       <c r="CM2" t="n">
-        <v>8.235916268216402</v>
+        <v>1.827852949733283</v>
       </c>
       <c r="CN2" t="n">
-        <v>8.235916268216402</v>
+        <v>0.5625087073662081</v>
       </c>
       <c r="CO2" t="n">
-        <v>8.235916268216402</v>
+        <v>2.986193557439884</v>
       </c>
       <c r="CP2" t="n">
-        <v>4.403425212402173</v>
+        <v>1.682711882058966</v>
       </c>
       <c r="CQ2" t="n">
-        <v>4.403425212402173</v>
+        <v>1.207606201421269</v>
       </c>
       <c r="CR2" t="n">
-        <v>4.403425212402173</v>
+        <v>0.6978887290991813</v>
       </c>
       <c r="CS2" t="n">
-        <v>4.403425212402173</v>
+        <v>1.60210781391204</v>
       </c>
       <c r="CT2" t="n">
-        <v>11.65622538147839</v>
+        <v>6.379492138601585</v>
       </c>
       <c r="CU2" t="n">
-        <v>11.65622538147839</v>
+        <v>3.870403376453598</v>
       </c>
       <c r="CV2" t="n">
-        <v>11.65622538147839</v>
+        <v>3.687376867371738</v>
       </c>
       <c r="CW2" t="n">
-        <v>11.65622538147839</v>
+        <v>1.211359782083931</v>
       </c>
       <c r="CX2" t="n">
-        <v>5.109138045739504</v>
+        <v>2.949359839648991</v>
       </c>
       <c r="CY2" t="n">
-        <v>5.109138045739504</v>
+        <v>2.198139705134757</v>
       </c>
       <c r="CZ2" t="n">
-        <v>5.109138045739504</v>
+        <v>1.480878210148284</v>
       </c>
       <c r="DA2" t="n">
-        <v>5.109138045739504</v>
+        <v>1.066605944643419</v>
       </c>
       <c r="DB2" t="n">
-        <v>6.733878104414119</v>
+        <v>3.05956891608967</v>
       </c>
       <c r="DC2" t="n">
-        <v>6.733878104414119</v>
+        <v>2.954348665212082</v>
       </c>
       <c r="DD2" t="n">
-        <v>6.733878104414119</v>
+        <v>2.008103924955496</v>
       </c>
       <c r="DE2" t="n">
-        <v>6.733878104414119</v>
+        <v>1.334896904523792</v>
       </c>
       <c r="DF2" t="n">
-        <v>4.2303277724783</v>
+        <v>2.213972539249219</v>
       </c>
       <c r="DG2" t="n">
-        <v>4.2303277724783</v>
+        <v>1.89718427602092</v>
       </c>
       <c r="DH2" t="n">
-        <v>4.2303277724783</v>
+        <v>1.637716373771159</v>
       </c>
       <c r="DI2" t="n">
-        <v>4.2303277724783</v>
+        <v>1.586112617633864</v>
       </c>
       <c r="DJ2" t="n">
-        <v>6.111882438747267</v>
+        <v>3.02418756885278</v>
       </c>
       <c r="DK2" t="n">
-        <v>6.111882438747267</v>
+        <v>3.188886506602614</v>
       </c>
       <c r="DL2" t="n">
-        <v>6.111882438747267</v>
+        <v>2.658564625829637</v>
       </c>
       <c r="DM2" t="n">
-        <v>6.111882438747267</v>
+        <v>1.682621343336702</v>
       </c>
       <c r="DN2" t="n">
-        <v>5.025118578845433</v>
+        <v>2.478259070749802</v>
       </c>
       <c r="DO2" t="n">
-        <v>5.025118578845433</v>
+        <v>1.983041953984996</v>
       </c>
       <c r="DP2" t="n">
-        <v>5.025118578845433</v>
+        <v>1.811410940354319</v>
       </c>
       <c r="DQ2" t="n">
-        <v>5.025118578845433</v>
+        <v>1.394544361721635</v>
       </c>
       <c r="DR2" t="n">
-        <v>3.728029065452467</v>
+        <v>1.818614241859829</v>
       </c>
       <c r="DS2" t="n">
-        <v>3.728029065452467</v>
+        <v>1.733011674298225</v>
       </c>
       <c r="DT2" t="n">
-        <v>3.728029065452467</v>
+        <v>2.71032205563027</v>
       </c>
       <c r="DU2" t="n">
-        <v>3.728029065452467</v>
+        <v>0.447894154083472</v>
       </c>
       <c r="DV2" t="n">
-        <v>4.549916668425563</v>
+        <v>2.203131036742743</v>
       </c>
       <c r="DW2" t="n">
-        <v>4.549916668425563</v>
+        <v>1.959453023913989</v>
       </c>
       <c r="DX2" t="n">
-        <v>4.549916668425563</v>
+        <v>2.562131406382532</v>
       </c>
       <c r="DY2" t="n">
-        <v>4.549916668425563</v>
+        <v>1.171636421847125</v>
       </c>
       <c r="DZ2" t="n">
-        <v>4.949619318139221</v>
+        <v>2.691421960573145</v>
       </c>
       <c r="EA2" t="n">
-        <v>4.949619318139221</v>
+        <v>1.408979948646794</v>
       </c>
       <c r="EB2" t="n">
-        <v>4.949619318139221</v>
+        <v>2.198938398484659</v>
       </c>
       <c r="EC2" t="n">
-        <v>4.949619318139221</v>
+        <v>0.7953311626153952</v>
       </c>
       <c r="ED2" t="n">
-        <v>5.043066674873618</v>
+        <v>2.545963700062983</v>
       </c>
       <c r="EE2" t="n">
-        <v>5.043066674873618</v>
+        <v>1.562470713993876</v>
       </c>
       <c r="EF2" t="n">
-        <v>5.043066674873618</v>
+        <v>2.285575126843332</v>
       </c>
       <c r="EG2" t="n">
-        <v>5.043066674873618</v>
+        <v>1.017649692778029</v>
       </c>
       <c r="EH2" t="n">
-        <v>5.110594904015435</v>
+        <v>2.725974369536307</v>
       </c>
       <c r="EI2" t="n">
-        <v>5.110594904015435</v>
+        <v>1.313260801754447</v>
       </c>
       <c r="EJ2" t="n">
-        <v>5.110594904015435</v>
+        <v>1.984831679813908</v>
       </c>
       <c r="EK2" t="n">
-        <v>5.110594904015435</v>
+        <v>1.183819502978078</v>
       </c>
       <c r="EL2" t="n">
-        <v>5.910770691477387</v>
+        <v>3.073676002816834</v>
       </c>
       <c r="EM2" t="n">
-        <v>5.910770691477387</v>
+        <v>2.092346706570996</v>
       </c>
       <c r="EN2" t="n">
-        <v>5.910770691477387</v>
+        <v>2.322755828695485</v>
       </c>
       <c r="EO2" t="n">
-        <v>5.910770691477387</v>
+        <v>1.685417326904668</v>
       </c>
     </row>
     <row r="3">
@@ -1601,436 +1601,436 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0812915854115337</v>
+        <v>0.05025795296319169</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0812915854115337</v>
+        <v>0.07290245429817044</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0812915854115337</v>
+        <v>0.09712068889725312</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0812915854115337</v>
+        <v>0.08874427423483544</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09295871421221302</v>
+        <v>0.07456026650848746</v>
       </c>
       <c r="G3" t="n">
-        <v>0.09295871421221302</v>
+        <v>0.07810369491517077</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09295871421221302</v>
+        <v>0.07197462611068306</v>
       </c>
       <c r="I3" t="n">
-        <v>0.09295871421221302</v>
+        <v>0.05680879953402451</v>
       </c>
       <c r="J3" t="n">
-        <v>0.08350974405608635</v>
+        <v>0.06167621947092417</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08350974405608635</v>
+        <v>0.08714395871911851</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08350974405608635</v>
+        <v>0.06962650750091548</v>
       </c>
       <c r="M3" t="n">
-        <v>0.08350974405608635</v>
+        <v>0.06819858826982617</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1071088531051336</v>
+        <v>0.08291778293141183</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1071088531051336</v>
+        <v>0.0634077472028145</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1071088531051336</v>
+        <v>0.06920508645662427</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1071088531051336</v>
+        <v>0.08234466444640498</v>
       </c>
       <c r="R3" t="n">
-        <v>0.08646517929120412</v>
+        <v>0.06146886238268912</v>
       </c>
       <c r="S3" t="n">
-        <v>0.08646517929120412</v>
+        <v>0.07895673633374756</v>
       </c>
       <c r="T3" t="n">
-        <v>0.08646517929120412</v>
+        <v>0.06122614091490397</v>
       </c>
       <c r="U3" t="n">
-        <v>0.08646517929120412</v>
+        <v>0.06585468972981179</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1052331054747297</v>
+        <v>0.07820866103016511</v>
       </c>
       <c r="W3" t="n">
-        <v>0.1052331054747297</v>
+        <v>0.07010475241083092</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1052331054747297</v>
+        <v>0.08136721142503966</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.1052331054747297</v>
+        <v>0.09375835247543862</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.1504763314694926</v>
+        <v>0.1473941626726116</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1504763314694926</v>
+        <v>0.1072411036044494</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1504763314694926</v>
+        <v>0.07556520252253618</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1504763314694926</v>
+        <v>0.1059382897760857</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.1136251803907806</v>
+        <v>0.1105360653562675</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.1136251803907806</v>
+        <v>0.08745166560084772</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.1136251803907806</v>
+        <v>0.06895856037522829</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.1136251803907806</v>
+        <v>0.08203629620338693</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.1179468917816864</v>
+        <v>0.1148391729851939</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.1179468917816864</v>
+        <v>0.08179377795531773</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.1179468917816864</v>
+        <v>0.06841663746212445</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.1179468917816864</v>
+        <v>0.06932458870951619</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.1043287088477731</v>
+        <v>0.1026900217349038</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.1043287088477731</v>
+        <v>0.08256430750223043</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.1043287088477731</v>
+        <v>0.0687537216845997</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.1043287088477731</v>
+        <v>0.08266456260084176</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.1156035161162625</v>
+        <v>0.1098172575905818</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.1156035161162625</v>
+        <v>0.09068216018456754</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1156035161162625</v>
+        <v>0.06744242546583323</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.1156035161162625</v>
+        <v>0.07643777804452023</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.09133498103481874</v>
+        <v>0.09132749702450371</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.09133498103481874</v>
+        <v>0.07680334740578298</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.09133498103481874</v>
+        <v>0.06076981991351627</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.09133498103481874</v>
+        <v>0.07922300703271912</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.1390713680315727</v>
+        <v>0.1005216245182852</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.1390713680315727</v>
+        <v>0.08500004175773479</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.1390713680315727</v>
+        <v>0.1087430761695387</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.1390713680315727</v>
+        <v>0.1035931041748051</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.1769723635227169</v>
+        <v>0.1371734070688724</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.1769723635227169</v>
+        <v>0.09250201532272739</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.1769723635227169</v>
+        <v>0.08193933001210274</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.1769723635227169</v>
+        <v>0.05090677700245116</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.1522508725477265</v>
+        <v>0.1159157942907578</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.1522508725477265</v>
+        <v>0.09423920401040897</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.1522508725477265</v>
+        <v>0.08758743415506376</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.1522508725477265</v>
+        <v>0.09432513844771195</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.1657560660752546</v>
+        <v>0.1359895886925275</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.1657560660752546</v>
+        <v>0.1022082170064109</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.1657560660752546</v>
+        <v>0.08872864075708087</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.1657560660752546</v>
+        <v>0.06548999391409183</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.1443208100905056</v>
+        <v>0.1131180644599448</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.1443208100905056</v>
+        <v>0.08643427495464295</v>
       </c>
       <c r="BP3" t="n">
-        <v>0.1443208100905056</v>
+        <v>0.082530887794241</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.1443208100905056</v>
+        <v>0.07862439982161096</v>
       </c>
       <c r="BR3" t="n">
-        <v>0.1528802605677464</v>
+        <v>0.122691890779556</v>
       </c>
       <c r="BS3" t="n">
-        <v>0.1528802605677464</v>
+        <v>0.09591526369121728</v>
       </c>
       <c r="BT3" t="n">
-        <v>0.1528802605677464</v>
+        <v>0.07961629555152316</v>
       </c>
       <c r="BU3" t="n">
-        <v>0.1528802605677464</v>
+        <v>0.07046810581942475</v>
       </c>
       <c r="BV3" t="n">
-        <v>0.09473147083974687</v>
+        <v>0.07002942002679391</v>
       </c>
       <c r="BW3" t="n">
-        <v>0.09473147083974687</v>
+        <v>0.08034220544659121</v>
       </c>
       <c r="BX3" t="n">
-        <v>0.09473147083974687</v>
+        <v>0.05563557788782392</v>
       </c>
       <c r="BY3" t="n">
-        <v>0.09473147083974687</v>
+        <v>0.1022684650603851</v>
       </c>
       <c r="BZ3" t="n">
-        <v>0.1022051231739105</v>
+        <v>0.06485529724393801</v>
       </c>
       <c r="CA3" t="n">
-        <v>0.1022051231739105</v>
+        <v>0.05298638100641795</v>
       </c>
       <c r="CB3" t="n">
-        <v>0.1022051231739105</v>
+        <v>0.03944280432804748</v>
       </c>
       <c r="CC3" t="n">
-        <v>0.1022051231739105</v>
+        <v>0.08813769384751069</v>
       </c>
       <c r="CD3" t="n">
-        <v>0.1231352132854484</v>
+        <v>0.1001919047617359</v>
       </c>
       <c r="CE3" t="n">
-        <v>0.1231352132854484</v>
+        <v>0.04676699189113709</v>
       </c>
       <c r="CF3" t="n">
-        <v>0.1231352132854484</v>
+        <v>0.03300364771767894</v>
       </c>
       <c r="CG3" t="n">
-        <v>0.1231352132854484</v>
+        <v>0.1034611481570828</v>
       </c>
       <c r="CH3" t="n">
-        <v>0.100502755328113</v>
+        <v>0.0642110718529878</v>
       </c>
       <c r="CI3" t="n">
-        <v>0.100502755328113</v>
+        <v>0.06864455312684958</v>
       </c>
       <c r="CJ3" t="n">
-        <v>0.100502755328113</v>
+        <v>0.03469399777008775</v>
       </c>
       <c r="CK3" t="n">
-        <v>0.100502755328113</v>
+        <v>0.07080890039466214</v>
       </c>
       <c r="CL3" t="n">
-        <v>0.1490594510693957</v>
+        <v>0.1277235311810787</v>
       </c>
       <c r="CM3" t="n">
-        <v>0.1490594510693957</v>
+        <v>0.0730185801483676</v>
       </c>
       <c r="CN3" t="n">
-        <v>0.1490594510693957</v>
+        <v>0.03071952934239786</v>
       </c>
       <c r="CO3" t="n">
-        <v>0.1490594510693957</v>
+        <v>0.0982869481930746</v>
       </c>
       <c r="CP3" t="n">
-        <v>0.1111989479547402</v>
+        <v>0.06919240879920663</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.1111989479547402</v>
+        <v>0.05515611217538918</v>
       </c>
       <c r="CR3" t="n">
-        <v>0.1111989479547402</v>
+        <v>0.03654238668912124</v>
       </c>
       <c r="CS3" t="n">
-        <v>0.1111989479547402</v>
+        <v>0.06698336017676576</v>
       </c>
       <c r="CT3" t="n">
-        <v>0.1719093317757094</v>
+        <v>0.1451153926648774</v>
       </c>
       <c r="CU3" t="n">
-        <v>0.1719093317757094</v>
+        <v>0.113306056417928</v>
       </c>
       <c r="CV3" t="n">
-        <v>0.1719093317757094</v>
+        <v>0.1104187104950531</v>
       </c>
       <c r="CW3" t="n">
-        <v>0.1719093317757094</v>
+        <v>0.05527764816564673</v>
       </c>
       <c r="CX3" t="n">
-        <v>0.1197568971799481</v>
+        <v>0.09759593141064471</v>
       </c>
       <c r="CY3" t="n">
-        <v>0.1197568971799481</v>
+        <v>0.08200765745899075</v>
       </c>
       <c r="CZ3" t="n">
-        <v>0.1197568971799481</v>
+        <v>0.06353775445361376</v>
       </c>
       <c r="DA3" t="n">
-        <v>0.1197568971799481</v>
+        <v>0.0504452018018775</v>
       </c>
       <c r="DB3" t="n">
-        <v>0.1363832734581067</v>
+        <v>0.09964594182771602</v>
       </c>
       <c r="DC3" t="n">
-        <v>0.1363832734581067</v>
+        <v>0.09768987486181535</v>
       </c>
       <c r="DD3" t="n">
-        <v>0.1363832734581067</v>
+        <v>0.07752320819904068</v>
       </c>
       <c r="DE3" t="n">
-        <v>0.1363832734581067</v>
+        <v>0.05917397785448819</v>
       </c>
       <c r="DF3" t="n">
-        <v>0.1089400195427153</v>
+        <v>0.08236998341144042</v>
       </c>
       <c r="DG3" t="n">
-        <v>0.1089400195427153</v>
+        <v>0.07478207533272019</v>
       </c>
       <c r="DH3" t="n">
-        <v>0.1089400195427153</v>
+        <v>0.06796700908089481</v>
       </c>
       <c r="DI3" t="n">
-        <v>0.1089400195427153</v>
+        <v>0.06653741920037048</v>
       </c>
       <c r="DJ3" t="n">
-        <v>0.1304439543304987</v>
+        <v>0.09899352387525862</v>
       </c>
       <c r="DK3" t="n">
-        <v>0.1304439543304987</v>
+        <v>0.1019862504970643</v>
       </c>
       <c r="DL3" t="n">
-        <v>0.1304439543304987</v>
+        <v>0.09191933943748953</v>
       </c>
       <c r="DM3" t="n">
-        <v>0.1304439543304987</v>
+        <v>0.06918996237927488</v>
       </c>
       <c r="DN3" t="n">
-        <v>0.1187881297899591</v>
+        <v>0.08818441961860013</v>
       </c>
       <c r="DO3" t="n">
-        <v>0.1187881297899591</v>
+        <v>0.07691219680783834</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.1187881297899591</v>
+        <v>0.07259445592491054</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0.1187881297899591</v>
+        <v>0.06098691112195542</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.1019642583053355</v>
+        <v>0.0727805500608274</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.1019642583053355</v>
+        <v>0.07053978705778174</v>
       </c>
       <c r="DT3" t="n">
-        <v>0.1019642583053355</v>
+        <v>0.09295977053611959</v>
       </c>
       <c r="DU3" t="n">
-        <v>0.1019642583053355</v>
+        <v>0.02540967584956455</v>
       </c>
       <c r="DV3" t="n">
-        <v>0.1130582779450457</v>
+        <v>0.08212206155774848</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.1130582779450457</v>
+        <v>0.07633271060708435</v>
       </c>
       <c r="DX3" t="n">
-        <v>0.1130582779450457</v>
+        <v>0.08994369507017752</v>
       </c>
       <c r="DY3" t="n">
-        <v>0.1130582779450457</v>
+        <v>0.05398158949944931</v>
       </c>
       <c r="DZ3" t="n">
-        <v>0.1179067376497009</v>
+        <v>0.09258141696121203</v>
       </c>
       <c r="EA3" t="n">
-        <v>0.1179067376497009</v>
+        <v>0.06141933757153062</v>
       </c>
       <c r="EB3" t="n">
-        <v>0.1179067376497009</v>
+        <v>0.08202597513626819</v>
       </c>
       <c r="EC3" t="n">
-        <v>0.1179067376497009</v>
+        <v>0.04047138386210292</v>
       </c>
       <c r="ED3" t="n">
-        <v>0.1189961353617026</v>
+        <v>0.08960759314505173</v>
       </c>
       <c r="EE3" t="n">
-        <v>0.1189961353617026</v>
+        <v>0.06587355901260494</v>
       </c>
       <c r="EF3" t="n">
-        <v>0.1189961353617026</v>
+        <v>0.08398806825863558</v>
       </c>
       <c r="EG3" t="n">
-        <v>0.1189961353617026</v>
+        <v>0.04873921949441251</v>
       </c>
       <c r="EH3" t="n">
-        <v>0.1197735847302488</v>
+        <v>0.09327175044403702</v>
       </c>
       <c r="EI3" t="n">
-        <v>0.1197735847302488</v>
+        <v>0.05850568079866791</v>
       </c>
       <c r="EJ3" t="n">
-        <v>0.1197735847302488</v>
+        <v>0.07695598872930187</v>
       </c>
       <c r="EK3" t="n">
-        <v>0.1197735847302488</v>
+        <v>0.05438142192237772</v>
       </c>
       <c r="EL3" t="n">
-        <v>0.1284190392309739</v>
+        <v>0.09990459382926642</v>
       </c>
       <c r="EM3" t="n">
-        <v>0.1284190392309739</v>
+        <v>0.079542828295037</v>
       </c>
       <c r="EN3" t="n">
-        <v>0.1284190392309739</v>
+        <v>0.08481535969905085</v>
       </c>
       <c r="EO3" t="n">
-        <v>0.1284190392309739</v>
+        <v>0.0692654763318068</v>
       </c>
     </row>
     <row r="4">
@@ -2040,436 +2040,436 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2150579431503619</v>
+        <v>0.2057140052586332</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2150579431503619</v>
+        <v>0.2189005934687788</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2150579431503619</v>
+        <v>0.1958893912892033</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2150579431503619</v>
+        <v>0.1942232575497569</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2084498214582717</v>
+        <v>0.2004834154055149</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2084498214582717</v>
+        <v>0.2032589035064503</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2084498214582717</v>
+        <v>0.1938603065525396</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2084498214582717</v>
+        <v>0.1817916947730303</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2007413104580969</v>
+        <v>0.190615706911966</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2007413104580969</v>
+        <v>0.1901077525752783</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2007413104580969</v>
+        <v>0.1791459139811063</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2007413104580969</v>
+        <v>0.1669601798454778</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1969015060166246</v>
+        <v>0.1836308610368612</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1969015060166246</v>
+        <v>0.1851402546473044</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1969015060166246</v>
+        <v>0.180079187442362</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1969015060166246</v>
+        <v>0.1774343740270617</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1986420459004891</v>
+        <v>0.1864796552316213</v>
       </c>
       <c r="S4" t="n">
-        <v>0.1986420459004891</v>
+        <v>0.190664705329183</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1986420459004891</v>
+        <v>0.1764341849494738</v>
       </c>
       <c r="U4" t="n">
-        <v>0.1986420459004891</v>
+        <v>0.1683549508026973</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1919611883468353</v>
+        <v>0.1796355746314554</v>
       </c>
       <c r="W4" t="n">
-        <v>0.1919611883468353</v>
+        <v>0.1828691665071634</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1919611883468353</v>
+        <v>0.1750459859746981</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.1919611883468353</v>
+        <v>0.1751948960758956</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2182854841355748</v>
+        <v>0.2180299146965831</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2182854841355748</v>
+        <v>0.2081479936180425</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.2182854841355748</v>
+        <v>0.2225780751651071</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.2182854841355748</v>
+        <v>0.2236793107203753</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1926866665343974</v>
+        <v>0.192197608604847</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.1926866665343974</v>
+        <v>0.1889476966092375</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.1926866665343974</v>
+        <v>0.2046130002600217</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.1926866665343974</v>
+        <v>0.1911760755665227</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.1875770227546162</v>
+        <v>0.1874857614111211</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.1875770227546162</v>
+        <v>0.177976126356275</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.1875770227546162</v>
+        <v>0.1889033293826375</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.1875770227546162</v>
+        <v>0.186467471276462</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.1824644409893553</v>
+        <v>0.1819634258977607</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.1824644409893553</v>
+        <v>0.1767627633503751</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.1824644409893553</v>
+        <v>0.1901364145416619</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.1824644409893553</v>
+        <v>0.1867028672648541</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.1788882316792169</v>
+        <v>0.1784092338772036</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.1788882316792169</v>
+        <v>0.1742347317401977</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.1788882316792169</v>
+        <v>0.183998338259406</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.1788882316792169</v>
+        <v>0.1856444499383295</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.1742628529171175</v>
+        <v>0.1734213286374899</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.1742628529171175</v>
+        <v>0.168943561535694</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.1742628529171175</v>
+        <v>0.1830531789899434</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.1742628529171175</v>
+        <v>0.1812455533357473</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.215445014129982</v>
+        <v>0.2088379285045527</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.215445014129982</v>
+        <v>0.2030065422422599</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.215445014129982</v>
+        <v>0.2037586334314477</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.215445014129982</v>
+        <v>0.1923732605267695</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.21184020494355</v>
+        <v>0.2022914022416213</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.21184020494355</v>
+        <v>0.2005761362044863</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.21184020494355</v>
+        <v>0.1937840255406868</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.21184020494355</v>
+        <v>0.1769164474750304</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.2043671409019974</v>
+        <v>0.1946863332284452</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.2043671409019974</v>
+        <v>0.1884541371310939</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.2043671409019974</v>
+        <v>0.1823827824357437</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.2043671409019974</v>
+        <v>0.1691073472216364</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.1964230588243261</v>
+        <v>0.1869956192230663</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.1964230588243261</v>
+        <v>0.1888135602146087</v>
       </c>
       <c r="BL4" t="n">
-        <v>0.1964230588243261</v>
+        <v>0.1763704943131265</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.1964230588243261</v>
+        <v>0.1668265648858046</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.1984387812337679</v>
+        <v>0.1895026397365492</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.1984387812337679</v>
+        <v>0.1851914232460911</v>
       </c>
       <c r="BP4" t="n">
-        <v>0.1984387812337679</v>
+        <v>0.1813384879687738</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0.1984387812337679</v>
+        <v>0.1724869297510723</v>
       </c>
       <c r="BR4" t="n">
-        <v>0.1875354613161436</v>
+        <v>0.179087641508249</v>
       </c>
       <c r="BS4" t="n">
-        <v>0.1875354613161436</v>
+        <v>0.1818008457363953</v>
       </c>
       <c r="BT4" t="n">
-        <v>0.1875354613161436</v>
+        <v>0.1722966416276191</v>
       </c>
       <c r="BU4" t="n">
-        <v>0.1875354613161436</v>
+        <v>0.1637360810514945</v>
       </c>
       <c r="BV4" t="n">
-        <v>0.2481381914017457</v>
+        <v>0.2461588661033159</v>
       </c>
       <c r="BW4" t="n">
-        <v>0.2481381914017457</v>
+        <v>0.2310977427960638</v>
       </c>
       <c r="BX4" t="n">
-        <v>0.2481381914017457</v>
+        <v>0.1984052441760236</v>
       </c>
       <c r="BY4" t="n">
-        <v>0.2481381914017457</v>
+        <v>0.2751715520930976</v>
       </c>
       <c r="BZ4" t="n">
-        <v>0.2121907060751635</v>
+        <v>0.1998179932502042</v>
       </c>
       <c r="CA4" t="n">
-        <v>0.2121907060751635</v>
+        <v>0.203155535281373</v>
       </c>
       <c r="CB4" t="n">
-        <v>0.2121907060751635</v>
+        <v>0.1902523847398566</v>
       </c>
       <c r="CC4" t="n">
-        <v>0.2121907060751635</v>
+        <v>0.209746949108145</v>
       </c>
       <c r="CD4" t="n">
-        <v>0.2313668525460821</v>
+        <v>0.2282393876776826</v>
       </c>
       <c r="CE4" t="n">
-        <v>0.2313668525460821</v>
+        <v>0.2124764916571692</v>
       </c>
       <c r="CF4" t="n">
-        <v>0.2313668525460821</v>
+        <v>0.1837294348085181</v>
       </c>
       <c r="CG4" t="n">
-        <v>0.2313668525460821</v>
+        <v>0.2169368473023272</v>
       </c>
       <c r="CH4" t="n">
-        <v>0.2082243450538763</v>
+        <v>0.19529295409859</v>
       </c>
       <c r="CI4" t="n">
-        <v>0.2082243450538763</v>
+        <v>0.2005139956561934</v>
       </c>
       <c r="CJ4" t="n">
-        <v>0.2082243450538763</v>
+        <v>0.1887974383343679</v>
       </c>
       <c r="CK4" t="n">
-        <v>0.2082243450538763</v>
+        <v>0.2016083985595185</v>
       </c>
       <c r="CL4" t="n">
-        <v>0.2253309872240834</v>
+        <v>0.2219677029006689</v>
       </c>
       <c r="CM4" t="n">
-        <v>0.2253309872240834</v>
+        <v>0.207566231775431</v>
       </c>
       <c r="CN4" t="n">
-        <v>0.2253309872240834</v>
+        <v>0.1788747417547938</v>
       </c>
       <c r="CO4" t="n">
-        <v>0.2253309872240834</v>
+        <v>0.205138275882444</v>
       </c>
       <c r="CP4" t="n">
-        <v>0.220207113087776</v>
+        <v>0.2049485750666427</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.220207113087776</v>
+        <v>0.1969985468043388</v>
       </c>
       <c r="CR4" t="n">
-        <v>0.220207113087776</v>
+        <v>0.1875919758754291</v>
       </c>
       <c r="CS4" t="n">
-        <v>0.220207113087776</v>
+        <v>0.1982693821618229</v>
       </c>
       <c r="CT4" t="n">
-        <v>0.185741750871033</v>
+        <v>0.1771839175399811</v>
       </c>
       <c r="CU4" t="n">
-        <v>0.185741750871033</v>
+        <v>0.180263706628237</v>
       </c>
       <c r="CV4" t="n">
-        <v>0.185741750871033</v>
+        <v>0.1888400317020981</v>
       </c>
       <c r="CW4" t="n">
-        <v>0.185741750871033</v>
+        <v>0.2044345391537007</v>
       </c>
       <c r="CX4" t="n">
-        <v>0.1796041828859807</v>
+        <v>0.1728784047894013</v>
       </c>
       <c r="CY4" t="n">
-        <v>0.1796041828859807</v>
+        <v>0.1704112278320128</v>
       </c>
       <c r="CZ4" t="n">
-        <v>0.1796041828859807</v>
+        <v>0.1685188762126314</v>
       </c>
       <c r="DA4" t="n">
-        <v>0.1796041828859807</v>
+        <v>0.1858416420135375</v>
       </c>
       <c r="DB4" t="n">
-        <v>0.1737895678848184</v>
+        <v>0.1662536041006467</v>
       </c>
       <c r="DC4" t="n">
-        <v>0.1737895678848184</v>
+        <v>0.1666040547564717</v>
       </c>
       <c r="DD4" t="n">
-        <v>0.1737895678848184</v>
+        <v>0.1649597467497391</v>
       </c>
       <c r="DE4" t="n">
-        <v>0.1737895678848184</v>
+        <v>0.1812128860032521</v>
       </c>
       <c r="DF4" t="n">
-        <v>0.1682467039370326</v>
+        <v>0.161244248870874</v>
       </c>
       <c r="DG4" t="n">
-        <v>0.1682467039370326</v>
+        <v>0.1646367349660497</v>
       </c>
       <c r="DH4" t="n">
-        <v>0.1682467039370326</v>
+        <v>0.1627086404802235</v>
       </c>
       <c r="DI4" t="n">
-        <v>0.1682467039370326</v>
+        <v>0.1702107077252334</v>
       </c>
       <c r="DJ4" t="n">
-        <v>0.1676443353423323</v>
+        <v>0.1601210542875644</v>
       </c>
       <c r="DK4" t="n">
-        <v>0.1676443353423323</v>
+        <v>0.1653034993094772</v>
       </c>
       <c r="DL4" t="n">
-        <v>0.1676443353423323</v>
+        <v>0.1628208839218308</v>
       </c>
       <c r="DM4" t="n">
-        <v>0.1676443353423323</v>
+        <v>0.1747666342116584</v>
       </c>
       <c r="DN4" t="n">
-        <v>0.1663726111730254</v>
+        <v>0.1579051932094161</v>
       </c>
       <c r="DO4" t="n">
-        <v>0.1663726111730254</v>
+        <v>0.1604603938944604</v>
       </c>
       <c r="DP4" t="n">
-        <v>0.1663726111730254</v>
+        <v>0.1572367185465308</v>
       </c>
       <c r="DQ4" t="n">
-        <v>0.1663726111730254</v>
+        <v>0.1645538182275434</v>
       </c>
       <c r="DR4" t="n">
-        <v>0.1931629971261058</v>
+        <v>0.1816332542281471</v>
       </c>
       <c r="DS4" t="n">
-        <v>0.1931629971261058</v>
+        <v>0.1878862060917557</v>
       </c>
       <c r="DT4" t="n">
-        <v>0.1931629971261058</v>
+        <v>0.1773208039753112</v>
       </c>
       <c r="DU4" t="n">
-        <v>0.1931629971261058</v>
+        <v>0.2007252163375169</v>
       </c>
       <c r="DV4" t="n">
-        <v>0.1991492636226608</v>
+        <v>0.1843635826381102</v>
       </c>
       <c r="DW4" t="n">
-        <v>0.1991492636226608</v>
+        <v>0.1947211134976572</v>
       </c>
       <c r="DX4" t="n">
-        <v>0.1991492636226608</v>
+        <v>0.1819964896678181</v>
       </c>
       <c r="DY4" t="n">
-        <v>0.1991492636226608</v>
+        <v>0.185481982745135</v>
       </c>
       <c r="DZ4" t="n">
-        <v>0.1843307277091877</v>
+        <v>0.177740310819857</v>
       </c>
       <c r="EA4" t="n">
-        <v>0.1843307277091877</v>
+        <v>0.1745206036399087</v>
       </c>
       <c r="EB4" t="n">
-        <v>0.1843307277091877</v>
+        <v>0.1727716835260744</v>
       </c>
       <c r="EC4" t="n">
-        <v>0.1843307277091877</v>
+        <v>0.1811447317257528</v>
       </c>
       <c r="ED4" t="n">
-        <v>0.1819505213962445</v>
+        <v>0.1707609511630386</v>
       </c>
       <c r="EE4" t="n">
-        <v>0.1819505213962445</v>
+        <v>0.1742556261526163</v>
       </c>
       <c r="EF4" t="n">
-        <v>0.1819505213962445</v>
+        <v>0.1748425555104986</v>
       </c>
       <c r="EG4" t="n">
-        <v>0.1819505213962445</v>
+        <v>0.1763170819965288</v>
       </c>
       <c r="EH4" t="n">
-        <v>0.1817999399413963</v>
+        <v>0.1700840596928667</v>
       </c>
       <c r="EI4" t="n">
-        <v>0.1817999399413963</v>
+        <v>0.1711738825007034</v>
       </c>
       <c r="EJ4" t="n">
-        <v>0.1817999399413963</v>
+        <v>0.1737714211613166</v>
       </c>
       <c r="EK4" t="n">
-        <v>0.1817999399413963</v>
+        <v>0.1753343118741707</v>
       </c>
       <c r="EL4" t="n">
-        <v>0.1801408191566706</v>
+        <v>0.1683716385571638</v>
       </c>
       <c r="EM4" t="n">
-        <v>0.1801408191566706</v>
+        <v>0.1667079897474424</v>
       </c>
       <c r="EN4" t="n">
-        <v>0.1801408191566706</v>
+        <v>0.1683094620503735</v>
       </c>
       <c r="EO4" t="n">
-        <v>0.1801408191566706</v>
+        <v>0.1711519555488492</v>
       </c>
     </row>
     <row r="5">
@@ -2479,436 +2479,436 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3779985255168981</v>
+        <v>0.2443098266450311</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3779985255168981</v>
+        <v>0.333039089309588</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3779985255168981</v>
+        <v>0.4957935100929892</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3779985255168981</v>
+        <v>0.4569188847638423</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4459524770129001</v>
+        <v>0.371902415756812</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4459524770129001</v>
+        <v>0.3842571890716325</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4459524770129001</v>
+        <v>0.3712705679188466</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4459524770129001</v>
+        <v>0.3124939211604313</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4160067694363206</v>
+        <v>0.3235631547373414</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4160067694363206</v>
+        <v>0.4583924513263157</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4160067694363206</v>
+        <v>0.388658082976197</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4160067694363206</v>
+        <v>0.4084721778147591</v>
       </c>
       <c r="N5" t="n">
-        <v>0.5439717312070244</v>
+        <v>0.45154601172821</v>
       </c>
       <c r="O5" t="n">
-        <v>0.5439717312070244</v>
+        <v>0.3424849302687168</v>
       </c>
       <c r="P5" t="n">
-        <v>0.5439717312070244</v>
+        <v>0.3843036357478832</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.5439717312070244</v>
+        <v>0.4640851858493105</v>
       </c>
       <c r="R5" t="n">
-        <v>0.4352813569717226</v>
+        <v>0.3296277135773354</v>
       </c>
       <c r="S5" t="n">
-        <v>0.4352813569717226</v>
+        <v>0.4141130168660664</v>
       </c>
       <c r="T5" t="n">
-        <v>0.4352813569717226</v>
+        <v>0.3470197169127828</v>
       </c>
       <c r="U5" t="n">
-        <v>0.4352813569717226</v>
+        <v>0.3911657448493441</v>
       </c>
       <c r="V5" t="n">
-        <v>0.548199906350833</v>
+        <v>0.4353740131408816</v>
       </c>
       <c r="W5" t="n">
-        <v>0.548199906350833</v>
+        <v>0.3833601571541299</v>
       </c>
       <c r="X5" t="n">
-        <v>0.548199906350833</v>
+        <v>0.4648333463459186</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.548199906350833</v>
+        <v>0.5351660041216147</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.6893556484774468</v>
+        <v>0.6760272455168811</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.6893556484774468</v>
+        <v>0.5152156489254461</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.6893556484774468</v>
+        <v>0.3394997574063949</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.6893556484774468</v>
+        <v>0.4736168465241769</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.5896888582609676</v>
+        <v>0.5751167569598984</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.5896888582609676</v>
+        <v>0.4628353092957063</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.5896888582609676</v>
+        <v>0.3370194478727936</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.5896888582609676</v>
+        <v>0.429113820650854</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.6287917893652769</v>
+        <v>0.6125221036565711</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.6287917893652769</v>
+        <v>0.4595772457232934</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.6287917893652769</v>
+        <v>0.3621780393480603</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.6287917893652769</v>
+        <v>0.3717784567729434</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.5717755650475455</v>
+        <v>0.5643442973677689</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.5717755650475455</v>
+        <v>0.467091065659419</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.5717755650475455</v>
+        <v>0.3616020731764386</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.5717755650475455</v>
+        <v>0.4427600058416616</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.6462332095918039</v>
+        <v>0.6155357276303723</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.6462332095918039</v>
+        <v>0.5204597228053484</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.6462332095918039</v>
+        <v>0.3665382312896273</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.6462332095918039</v>
+        <v>0.4117428669152923</v>
       </c>
       <c r="AT5" t="n">
-        <v>0.5241219198807636</v>
+        <v>0.5266220582095155</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.5241219198807636</v>
+        <v>0.4546094962580517</v>
       </c>
       <c r="AV5" t="n">
-        <v>0.5241219198807636</v>
+        <v>0.331979047011551</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.5241219198807636</v>
+        <v>0.4371031761864132</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.6455074794521276</v>
+        <v>0.4813379697744596</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.6455074794521276</v>
+        <v>0.4187059235573756</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.6455074794521276</v>
+        <v>0.5336857356089605</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.6455074794521276</v>
+        <v>0.5385005373986976</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.8354049863663771</v>
+        <v>0.6780980582903344</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.8354049863663771</v>
+        <v>0.4611815596468668</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.8354049863663771</v>
+        <v>0.4228384139687449</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.8354049863663771</v>
+        <v>0.287744738994016</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.7449870457439985</v>
+        <v>0.5953976962252511</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.7449870457439985</v>
+        <v>0.5000643946853424</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.7449870457439985</v>
+        <v>0.4802395981973913</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.7449870457439985</v>
+        <v>0.5577826155837394</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.8438727462415755</v>
+        <v>0.7272340884644262</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.8438727462415755</v>
+        <v>0.5413182024121537</v>
       </c>
       <c r="BL5" t="n">
-        <v>0.8438727462415755</v>
+        <v>0.5030809779302025</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.8438727462415755</v>
+        <v>0.3925633424084514</v>
       </c>
       <c r="BN5" t="n">
-        <v>0.7272812763372626</v>
+        <v>0.5969207849410649</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.7272812763372626</v>
+        <v>0.4667293627296391</v>
       </c>
       <c r="BP5" t="n">
-        <v>0.7272812763372626</v>
+        <v>0.4551206349997397</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.7272812763372626</v>
+        <v>0.455828160052934</v>
       </c>
       <c r="BR5" t="n">
-        <v>0.8152072119844249</v>
+        <v>0.6850941234485166</v>
       </c>
       <c r="BS5" t="n">
-        <v>0.8152072119844249</v>
+        <v>0.5275842546425278</v>
       </c>
       <c r="BT5" t="n">
-        <v>0.8152072119844249</v>
+        <v>0.4620884934228496</v>
       </c>
       <c r="BU5" t="n">
-        <v>0.8152072119844249</v>
+        <v>0.4303761600185285</v>
       </c>
       <c r="BV5" t="n">
-        <v>0.3817690066353905</v>
+        <v>0.2844887171254749</v>
       </c>
       <c r="BW5" t="n">
-        <v>0.3817690066353905</v>
+        <v>0.347654652419044</v>
       </c>
       <c r="BX5" t="n">
-        <v>0.3817690066353905</v>
+        <v>0.2804138475214116</v>
       </c>
       <c r="BY5" t="n">
-        <v>0.3817690066353905</v>
+        <v>0.3716534804651067</v>
       </c>
       <c r="BZ5" t="n">
-        <v>0.4816663512948903</v>
+        <v>0.3245718575640422</v>
       </c>
       <c r="CA5" t="n">
-        <v>0.4816663512948903</v>
+        <v>0.2608168216191163</v>
       </c>
       <c r="CB5" t="n">
-        <v>0.4816663512948903</v>
+        <v>0.2073183176230877</v>
       </c>
       <c r="CC5" t="n">
-        <v>0.4816663512948903</v>
+        <v>0.4202096584588085</v>
       </c>
       <c r="CD5" t="n">
-        <v>0.5322076690347125</v>
+        <v>0.4389772763639986</v>
       </c>
       <c r="CE5" t="n">
-        <v>0.5322076690347125</v>
+        <v>0.2201043114294057</v>
       </c>
       <c r="CF5" t="n">
-        <v>0.5322076690347125</v>
+        <v>0.1796317925436128</v>
       </c>
       <c r="CG5" t="n">
-        <v>0.5322076690347125</v>
+        <v>0.4769182803366616</v>
       </c>
       <c r="CH5" t="n">
-        <v>0.4826657291303224</v>
+        <v>0.3287935919110121</v>
       </c>
       <c r="CI5" t="n">
-        <v>0.4826657291303224</v>
+        <v>0.3423429516837785</v>
       </c>
       <c r="CJ5" t="n">
-        <v>0.4826657291303224</v>
+        <v>0.1837630747332667</v>
       </c>
       <c r="CK5" t="n">
-        <v>0.4826657291303224</v>
+        <v>0.3512199933166874</v>
       </c>
       <c r="CL5" t="n">
-        <v>0.6615133271535421</v>
+        <v>0.5754149342989565</v>
       </c>
       <c r="CM5" t="n">
-        <v>0.6615133271535421</v>
+        <v>0.3517844859628588</v>
       </c>
       <c r="CN5" t="n">
-        <v>0.6615133271535421</v>
+        <v>0.1717376586600974</v>
       </c>
       <c r="CO5" t="n">
-        <v>0.6615133271535421</v>
+        <v>0.4791253498172064</v>
       </c>
       <c r="CP5" t="n">
-        <v>0.5049743688816063</v>
+        <v>0.3376086356136287</v>
       </c>
       <c r="CQ5" t="n">
-        <v>0.5049743688816063</v>
+        <v>0.2799823301751097</v>
       </c>
       <c r="CR5" t="n">
-        <v>0.5049743688816063</v>
+        <v>0.1947971735922612</v>
       </c>
       <c r="CS5" t="n">
-        <v>0.5049743688816063</v>
+        <v>0.3378401619373357</v>
       </c>
       <c r="CT5" t="n">
-        <v>0.9255287568333097</v>
+        <v>0.8190099568835443</v>
       </c>
       <c r="CU5" t="n">
-        <v>0.9255287568333097</v>
+        <v>0.6285572317205388</v>
       </c>
       <c r="CV5" t="n">
-        <v>0.9255287568333097</v>
+        <v>0.5847208851841468</v>
       </c>
       <c r="CW5" t="n">
-        <v>0.9255287568333097</v>
+        <v>0.2703929012899681</v>
       </c>
       <c r="CX5" t="n">
-        <v>0.6667823391172029</v>
+        <v>0.5645351224147115</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.6667823391172029</v>
+        <v>0.4812338864187511</v>
       </c>
       <c r="CZ5" t="n">
-        <v>0.6667823391172029</v>
+        <v>0.3770364239400931</v>
       </c>
       <c r="DA5" t="n">
-        <v>0.6667823391172029</v>
+        <v>0.2714418644568522</v>
       </c>
       <c r="DB5" t="n">
-        <v>0.7847609906510427</v>
+        <v>0.599361092751964</v>
       </c>
       <c r="DC5" t="n">
-        <v>0.7847609906510427</v>
+        <v>0.5863595277114383</v>
       </c>
       <c r="DD5" t="n">
-        <v>0.7847609906510427</v>
+        <v>0.4699522745791516</v>
       </c>
       <c r="DE5" t="n">
-        <v>0.7847609906510427</v>
+        <v>0.3265439845896292</v>
       </c>
       <c r="DF5" t="n">
-        <v>0.6475016567545164</v>
+        <v>0.5108398221222956</v>
       </c>
       <c r="DG5" t="n">
-        <v>0.6475016567545164</v>
+        <v>0.4542247229826395</v>
       </c>
       <c r="DH5" t="n">
-        <v>0.6475016567545164</v>
+        <v>0.4177221866048098</v>
       </c>
       <c r="DI5" t="n">
-        <v>0.6475016567545164</v>
+        <v>0.3909120647555267</v>
       </c>
       <c r="DJ5" t="n">
-        <v>0.7780993856078117</v>
+        <v>0.6182417691147242</v>
       </c>
       <c r="DK5" t="n">
-        <v>0.7780993856078117</v>
+        <v>0.6169636512420595</v>
       </c>
       <c r="DL5" t="n">
-        <v>0.7780993856078117</v>
+        <v>0.5645426877894816</v>
       </c>
       <c r="DM5" t="n">
-        <v>0.7780993856078117</v>
+        <v>0.3958991525549408</v>
       </c>
       <c r="DN5" t="n">
-        <v>0.7139884921708718</v>
+        <v>0.5584643406987174</v>
       </c>
       <c r="DO5" t="n">
-        <v>0.7139884921708718</v>
+        <v>0.4793219992867885</v>
       </c>
       <c r="DP5" t="n">
-        <v>0.7139884921708718</v>
+        <v>0.4616889527838102</v>
       </c>
       <c r="DQ5" t="n">
-        <v>0.7139884921708718</v>
+        <v>0.3706198481376065</v>
       </c>
       <c r="DR5" t="n">
-        <v>0.5278664124204312</v>
+        <v>0.400700578592336</v>
       </c>
       <c r="DS5" t="n">
-        <v>0.5278664124204312</v>
+        <v>0.3754388814649495</v>
       </c>
       <c r="DT5" t="n">
-        <v>0.5278664124204312</v>
+        <v>0.5242462725866198</v>
       </c>
       <c r="DU5" t="n">
-        <v>0.5278664124204312</v>
+        <v>0.1265893559025414</v>
       </c>
       <c r="DV5" t="n">
-        <v>0.5677062314388648</v>
+        <v>0.4454353749403265</v>
       </c>
       <c r="DW5" t="n">
-        <v>0.5677062314388648</v>
+        <v>0.3920104463042871</v>
       </c>
       <c r="DX5" t="n">
-        <v>0.5677062314388648</v>
+        <v>0.4942056587703624</v>
       </c>
       <c r="DY5" t="n">
-        <v>0.5677062314388648</v>
+        <v>0.2910341408934782</v>
       </c>
       <c r="DZ5" t="n">
-        <v>0.6396477630995868</v>
+        <v>0.5208802467721854</v>
       </c>
       <c r="EA5" t="n">
-        <v>0.6396477630995868</v>
+        <v>0.3519317277761551</v>
       </c>
       <c r="EB5" t="n">
-        <v>0.6396477630995868</v>
+        <v>0.4747651551585939</v>
       </c>
       <c r="EC5" t="n">
-        <v>0.6396477630995868</v>
+        <v>0.2234201540201305</v>
       </c>
       <c r="ED5" t="n">
-        <v>0.6540027170494205</v>
+        <v>0.5247545913438751</v>
       </c>
       <c r="EE5" t="n">
-        <v>0.6540027170494205</v>
+        <v>0.3780283051229099</v>
       </c>
       <c r="EF5" t="n">
-        <v>0.6540027170494205</v>
+        <v>0.4803639938424055</v>
       </c>
       <c r="EG5" t="n">
-        <v>0.6540027170494205</v>
+        <v>0.2764293677193004</v>
       </c>
       <c r="EH5" t="n">
-        <v>0.6588208157211609</v>
+        <v>0.5483861956991424</v>
       </c>
       <c r="EI5" t="n">
-        <v>0.6588208157211609</v>
+        <v>0.3417909317937419</v>
       </c>
       <c r="EJ5" t="n">
-        <v>0.6588208157211609</v>
+        <v>0.4428575666528135</v>
       </c>
       <c r="EK5" t="n">
-        <v>0.6588208157211609</v>
+        <v>0.3101584700740419</v>
       </c>
       <c r="EL5" t="n">
-        <v>0.7128813992973259</v>
+        <v>0.5933576146516376</v>
       </c>
       <c r="EM5" t="n">
-        <v>0.7128813992973259</v>
+        <v>0.4771386687317267</v>
       </c>
       <c r="EN5" t="n">
-        <v>0.7128813992973259</v>
+        <v>0.5039250833899427</v>
       </c>
       <c r="EO5" t="n">
-        <v>0.7128813992973259</v>
+        <v>0.404701635512645</v>
       </c>
     </row>
     <row r="6">
@@ -2918,436 +2918,436 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.5061547306553378</v>
+        <v>-0.4744768554083818</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.5061547306553378</v>
+        <v>-0.4243217500465033</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5061547306553378</v>
+        <v>-0.3589945677748207</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.5061547306553378</v>
+        <v>-0.3737818933449653</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.4257966510215609</v>
+        <v>-0.3925535577012682</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.4257966510215609</v>
+        <v>-0.479581734310413</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.4257966510215609</v>
+        <v>-0.4835013648903937</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.4257966510215609</v>
+        <v>-0.4830991860737468</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.4421987289573991</v>
+        <v>-0.442198728957399</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.4421987289573991</v>
+        <v>-0.444023073271784</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.4421987289573991</v>
+        <v>-0.4462568251409467</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.4421987289573991</v>
+        <v>-0.3912868585517444</v>
       </c>
       <c r="N6" t="n">
         <v>-0.3530894921614827</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.3530894921614827</v>
+        <v>-0.4661413231029029</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.3530894921614827</v>
+        <v>-0.4796519235570331</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.3530894921614827</v>
+        <v>-0.4074250475293928</v>
       </c>
       <c r="R6" t="n">
         <v>-0.4431614635843616</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.4431614635843616</v>
+        <v>-0.4727357914381067</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.4431614635843616</v>
+        <v>-0.4604405018055654</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.4431614635843616</v>
+        <v>-0.4252135927864323</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.365930157512839</v>
+        <v>-0.3659301575128386</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.365930157512839</v>
+        <v>-0.4403302962311643</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.365930157512839</v>
+        <v>-0.4574955855052214</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.365930157512839</v>
+        <v>-0.3709921302289015</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.3228682503037497</v>
+        <v>-0.3228682503037499</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.3228682503037497</v>
+        <v>-0.2980877315236105</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.3228682503037497</v>
+        <v>-0.3276596730205168</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.3228682503037497</v>
+        <v>-0.4024296333857031</v>
       </c>
       <c r="AD6" t="n">
         <v>-0.4085479270002076</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.4085479270002076</v>
+        <v>-0.343314351934211</v>
       </c>
       <c r="AF6" t="n">
-        <v>-0.4085479270002076</v>
+        <v>-0.4595821733755375</v>
       </c>
       <c r="AG6" t="n">
-        <v>-0.4085479270002076</v>
+        <v>-0.4002041191788562</v>
       </c>
       <c r="AH6" t="n">
-        <v>-0.3884951363823687</v>
+        <v>-0.3884951363823685</v>
       </c>
       <c r="AI6" t="n">
-        <v>-0.3884951363823687</v>
+        <v>-0.355746450166844</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-0.3884951363823687</v>
+        <v>-0.4238950206165529</v>
       </c>
       <c r="AK6" t="n">
-        <v>-0.3884951363823687</v>
+        <v>-0.4546128943595502</v>
       </c>
       <c r="AL6" t="n">
-        <v>-0.3968656336808146</v>
+        <v>-0.3968656336808142</v>
       </c>
       <c r="AM6" t="n">
-        <v>-0.3968656336808146</v>
+        <v>-0.3584880971539443</v>
       </c>
       <c r="AN6" t="n">
-        <v>-0.3968656336808146</v>
+        <v>-0.4163784855841275</v>
       </c>
       <c r="AO6" t="n">
-        <v>-0.3968656336808146</v>
+        <v>-0.413880745187569</v>
       </c>
       <c r="AP6" t="n">
-        <v>-0.3861405539481917</v>
+        <v>-0.3861405539481916</v>
       </c>
       <c r="AQ6" t="n">
-        <v>-0.3861405539481917</v>
+        <v>-0.3393257530452836</v>
       </c>
       <c r="AR6" t="n">
-        <v>-0.3861405539481917</v>
+        <v>-0.4263723787536947</v>
       </c>
       <c r="AS6" t="n">
-        <v>-0.3861405539481917</v>
+        <v>-0.451682848674827</v>
       </c>
       <c r="AT6" t="n">
-        <v>-0.4294323469835482</v>
+        <v>-0.4294323469835479</v>
       </c>
       <c r="AU6" t="n">
-        <v>-0.4294323469835482</v>
+        <v>-0.383592558276004</v>
       </c>
       <c r="AV6" t="n">
-        <v>-0.4294323469835482</v>
+        <v>-0.4662549349223727</v>
       </c>
       <c r="AW6" t="n">
-        <v>-0.4294323469835482</v>
+        <v>-0.4649829341141298</v>
       </c>
       <c r="AX6" t="n">
         <v>-0.4577144551053585</v>
       </c>
       <c r="AY6" t="n">
-        <v>-0.4577144551053585</v>
+        <v>-0.4257754978388464</v>
       </c>
       <c r="AZ6" t="n">
-        <v>-0.4577144551053585</v>
+        <v>-0.384279615461348</v>
       </c>
       <c r="BA6" t="n">
-        <v>-0.4577144551053585</v>
+        <v>-0.3052461540836791</v>
       </c>
       <c r="BB6" t="n">
         <v>-0.3382265564094655</v>
       </c>
       <c r="BC6" t="n">
-        <v>-0.3382265564094655</v>
+        <v>-0.3639920926084612</v>
       </c>
       <c r="BD6" t="n">
-        <v>-0.3382265564094655</v>
+        <v>-0.3889459820640061</v>
       </c>
       <c r="BE6" t="n">
-        <v>-0.3382265564094655</v>
+        <v>-0.4431991254542811</v>
       </c>
       <c r="BF6" t="n">
         <v>-0.3957694572692457</v>
       </c>
       <c r="BG6" t="n">
-        <v>-0.3957694572692457</v>
+        <v>-0.3674525522288771</v>
       </c>
       <c r="BH6" t="n">
-        <v>-0.3957694572692457</v>
+        <v>-0.4125391414777935</v>
       </c>
       <c r="BI6" t="n">
-        <v>-0.3957694572692457</v>
+        <v>-0.3121279303464082</v>
       </c>
       <c r="BJ6" t="n">
-        <v>-0.3923185056843573</v>
+        <v>-0.3923185056843571</v>
       </c>
       <c r="BK6" t="n">
-        <v>-0.3923185056843573</v>
+        <v>-0.3484732616943526</v>
       </c>
       <c r="BL6" t="n">
-        <v>-0.3923185056843573</v>
+        <v>-0.4003108955481066</v>
       </c>
       <c r="BM6" t="n">
-        <v>-0.3923185056843573</v>
+        <v>-0.3559589076040307</v>
       </c>
       <c r="BN6" t="n">
         <v>-0.3722264658311051</v>
       </c>
       <c r="BO6" t="n">
-        <v>-0.3722264658311051</v>
+        <v>-0.3601100009667118</v>
       </c>
       <c r="BP6" t="n">
-        <v>-0.3722264658311051</v>
+        <v>-0.4211418703673542</v>
       </c>
       <c r="BQ6" t="n">
-        <v>-0.3722264658311051</v>
+        <v>-0.3365335330011847</v>
       </c>
       <c r="BR6" t="n">
-        <v>-0.3669212371587891</v>
+        <v>-0.3669212371587888</v>
       </c>
       <c r="BS6" t="n">
-        <v>-0.3669212371587891</v>
+        <v>-0.3723037416529474</v>
       </c>
       <c r="BT6" t="n">
-        <v>-0.3669212371587891</v>
+        <v>-0.4171697362143048</v>
       </c>
       <c r="BU6" t="n">
-        <v>-0.3669212371587891</v>
+        <v>-0.3481310448079924</v>
       </c>
       <c r="BV6" t="n">
-        <v>-0.5620928363606261</v>
+        <v>-0.5620928363606259</v>
       </c>
       <c r="BW6" t="n">
-        <v>-0.5620928363606261</v>
+        <v>-0.4513533822982601</v>
       </c>
       <c r="BX6" t="n">
-        <v>-0.5620928363606261</v>
+        <v>-0.4672648600241183</v>
       </c>
       <c r="BY6" t="n">
-        <v>-0.5620928363606261</v>
+        <v>-0.4710870733445339</v>
       </c>
       <c r="BZ6" t="n">
         <v>-0.3865669889515791</v>
       </c>
       <c r="CA6" t="n">
-        <v>-0.3865669889515791</v>
+        <v>-0.3512486399100397</v>
       </c>
       <c r="CB6" t="n">
-        <v>-0.3865669889515791</v>
+        <v>-0.3905685456691773</v>
       </c>
       <c r="CC6" t="n">
-        <v>-0.3865669889515791</v>
+        <v>-0.4248046903623074</v>
       </c>
       <c r="CD6" t="n">
-        <v>-0.4498584133752966</v>
+        <v>-0.4498584133752963</v>
       </c>
       <c r="CE6" t="n">
-        <v>-0.4498584133752966</v>
+        <v>-0.438491133345094</v>
       </c>
       <c r="CF6" t="n">
-        <v>-0.4498584133752966</v>
+        <v>-0.4526767650663317</v>
       </c>
       <c r="CG6" t="n">
-        <v>-0.4498584133752966</v>
+        <v>-0.4048505259602512</v>
       </c>
       <c r="CH6" t="n">
-        <v>-0.3560798792954976</v>
+        <v>-0.3560798792954974</v>
       </c>
       <c r="CI6" t="n">
-        <v>-0.3560798792954976</v>
+        <v>-0.3166854591611854</v>
       </c>
       <c r="CJ6" t="n">
-        <v>-0.3560798792954976</v>
+        <v>-0.4146265919634657</v>
       </c>
       <c r="CK6" t="n">
-        <v>-0.3560798792954976</v>
+        <v>-0.4046031121905306</v>
       </c>
       <c r="CL6" t="n">
-        <v>-0.4301160760386105</v>
+        <v>-0.4301160760386107</v>
       </c>
       <c r="CM6" t="n">
-        <v>-0.4301160760386105</v>
+        <v>-0.3552998775270576</v>
       </c>
       <c r="CN6" t="n">
-        <v>-0.4301160760386105</v>
+        <v>-0.4184201690258433</v>
       </c>
       <c r="CO6" t="n">
-        <v>-0.4301160760386105</v>
+        <v>-0.4175436102402251</v>
       </c>
       <c r="CP6" t="n">
-        <v>-0.3592914489991087</v>
+        <v>-0.3592914489991086</v>
       </c>
       <c r="CQ6" t="n">
-        <v>-0.3592914489991087</v>
+        <v>-0.3483788950764338</v>
       </c>
       <c r="CR6" t="n">
-        <v>-0.3592914489991087</v>
+        <v>-0.4080536017377202</v>
       </c>
       <c r="CS6" t="n">
-        <v>-0.3592914489991087</v>
+        <v>-0.4051902407429661</v>
       </c>
       <c r="CT6" t="n">
-        <v>-0.4279143970599454</v>
+        <v>-0.4279143970599455</v>
       </c>
       <c r="CU6" t="n">
-        <v>-0.4279143970599454</v>
+        <v>-0.4533245623508346</v>
       </c>
       <c r="CV6" t="n">
-        <v>-0.4279143970599454</v>
+        <v>-0.502087915855463</v>
       </c>
       <c r="CW6" t="n">
-        <v>-0.4279143970599454</v>
+        <v>-0.57037398520349</v>
       </c>
       <c r="CX6" t="n">
-        <v>-0.4715548393187676</v>
+        <v>-0.4715548393187677</v>
       </c>
       <c r="CY6" t="n">
-        <v>-0.4715548393187676</v>
+        <v>-0.5105372015489202</v>
       </c>
       <c r="CZ6" t="n">
-        <v>-0.4715548393187676</v>
+        <v>-0.5259777705913165</v>
       </c>
       <c r="DA6" t="n">
-        <v>-0.4715548393187676</v>
+        <v>-0.5540725489384561</v>
       </c>
       <c r="DB6" t="n">
-        <v>-0.4802793040235313</v>
+        <v>-0.4802793040235311</v>
       </c>
       <c r="DC6" t="n">
-        <v>-0.4802793040235313</v>
+        <v>-0.480546280311394</v>
       </c>
       <c r="DD6" t="n">
-        <v>-0.4802793040235313</v>
+        <v>-0.4456975532709364</v>
       </c>
       <c r="DE6" t="n">
-        <v>-0.4802793040235313</v>
+        <v>-0.4914513448801968</v>
       </c>
       <c r="DF6" t="n">
-        <v>-0.4352553451113081</v>
+        <v>-0.4352553451113083</v>
       </c>
       <c r="DG6" t="n">
-        <v>-0.4352553451113081</v>
+        <v>-0.4586877916273334</v>
       </c>
       <c r="DH6" t="n">
-        <v>-0.4352553451113081</v>
+        <v>-0.4551791463004119</v>
       </c>
       <c r="DI6" t="n">
-        <v>-0.4352553451113081</v>
+        <v>-0.46490964732194</v>
       </c>
       <c r="DJ6" t="n">
-        <v>-0.4923132610868639</v>
+        <v>-0.492313261086864</v>
       </c>
       <c r="DK6" t="n">
-        <v>-0.4923132610868639</v>
+        <v>-0.4827711319418351</v>
       </c>
       <c r="DL6" t="n">
-        <v>-0.4923132610868639</v>
+        <v>-0.432124172966504</v>
       </c>
       <c r="DM6" t="n">
-        <v>-0.4923132610868639</v>
+        <v>-0.4676153157769649</v>
       </c>
       <c r="DN6" t="n">
-        <v>-0.4329861439652393</v>
+        <v>-0.4329861439652389</v>
       </c>
       <c r="DO6" t="n">
-        <v>-0.4329861439652393</v>
+        <v>-0.4655283115564157</v>
       </c>
       <c r="DP6" t="n">
-        <v>-0.4329861439652393</v>
+        <v>-0.4421494461542548</v>
       </c>
       <c r="DQ6" t="n">
-        <v>-0.4329861439652393</v>
+        <v>-0.4737891762034994</v>
       </c>
       <c r="DR6" t="n">
         <v>-0.4495180092307239</v>
       </c>
       <c r="DS6" t="n">
-        <v>-0.4495180092307239</v>
+        <v>-0.5016341294112989</v>
       </c>
       <c r="DT6" t="n">
-        <v>-0.4495180092307239</v>
+        <v>-0.5180538556808303</v>
       </c>
       <c r="DU6" t="n">
-        <v>-0.4495180092307239</v>
+        <v>-0.6744283489901572</v>
       </c>
       <c r="DV6" t="n">
-        <v>-0.439985168640494</v>
+        <v>-0.4399851686404942</v>
       </c>
       <c r="DW6" t="n">
-        <v>-0.439985168640494</v>
+        <v>-0.5253338218349384</v>
       </c>
       <c r="DX6" t="n">
-        <v>-0.439985168640494</v>
+        <v>-0.4438744474348715</v>
       </c>
       <c r="DY6" t="n">
-        <v>-0.439985168640494</v>
+        <v>-0.5460871412350945</v>
       </c>
       <c r="DZ6" t="n">
         <v>-0.4738465415363986</v>
       </c>
       <c r="EA6" t="n">
-        <v>-0.4738465415363986</v>
+        <v>-0.4721287422670613</v>
       </c>
       <c r="EB6" t="n">
-        <v>-0.4738465415363986</v>
+        <v>-0.4626621766599456</v>
       </c>
       <c r="EC6" t="n">
-        <v>-0.4738465415363986</v>
+        <v>-0.5547771303887097</v>
       </c>
       <c r="ED6" t="n">
-        <v>-0.3988038196159307</v>
+        <v>-0.3988038196159306</v>
       </c>
       <c r="EE6" t="n">
-        <v>-0.3988038196159307</v>
+        <v>-0.4798964093205661</v>
       </c>
       <c r="EF6" t="n">
-        <v>-0.3988038196159307</v>
+        <v>-0.4207398942038617</v>
       </c>
       <c r="EG6" t="n">
-        <v>-0.3988038196159307</v>
+        <v>-0.5104955878037143</v>
       </c>
       <c r="EH6" t="n">
-        <v>-0.430791909168837</v>
+        <v>-0.4307919091688374</v>
       </c>
       <c r="EI6" t="n">
-        <v>-0.430791909168837</v>
+        <v>-0.4674390590364241</v>
       </c>
       <c r="EJ6" t="n">
-        <v>-0.430791909168837</v>
+        <v>-0.4703426209965295</v>
       </c>
       <c r="EK6" t="n">
-        <v>-0.430791909168837</v>
+        <v>-0.5117853756707318</v>
       </c>
       <c r="EL6" t="n">
-        <v>-0.3971052407553111</v>
+        <v>-0.397105240755311</v>
       </c>
       <c r="EM6" t="n">
-        <v>-0.3971052407553111</v>
+        <v>-0.4240383310288325</v>
       </c>
       <c r="EN6" t="n">
-        <v>-0.3971052407553111</v>
+        <v>-0.4229555064112622</v>
       </c>
       <c r="EO6" t="n">
-        <v>-0.3971052407553111</v>
+        <v>-0.4863714286627516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>